<commit_message>
se agrega xls de mediciones
</commit_message>
<xml_diff>
--- a/mediciones4.xlsx
+++ b/mediciones4.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Datos\UTN 2022\DDS 2022\DDS-2022-K3002-HuellaCarbonoG3\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C31ADCB-BB5B-48BD-9597-E294B4E5AE0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Hoja1" sheetId="1" r:id="rId4"/>
+    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mjYkrEKyAvl/YjKAI2fYBrikuNswg=="/>
@@ -90,21 +99,25 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
-    <font/>
     <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
@@ -115,7 +128,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -131,76 +144,93 @@
     </fill>
   </fills>
   <borders count="6">
-    <border/>
     <border>
       <left/>
       <right/>
       <top/>
-    </border>
-    <border>
-      <left/>
-      <top/>
       <bottom/>
-    </border>
-    <border>
-      <right/>
-      <top/>
-      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
+      <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="11">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="4" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="17" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -390,181 +420,204 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F991"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="25.29"/>
-    <col customWidth="1" min="2" max="2" width="24.57"/>
-    <col customWidth="1" min="3" max="4" width="10.71"/>
-    <col customWidth="1" min="5" max="5" width="20.71"/>
-    <col customWidth="1" min="6" max="6" width="22.71"/>
-    <col customWidth="1" min="7" max="26" width="10.71"/>
+    <col min="1" max="1" width="25.28515625" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" customWidth="1"/>
+    <col min="3" max="4" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" customWidth="1"/>
+    <col min="7" max="26" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="5" t="s">
+      <c r="D1" s="9"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="4" t="s">
+    <row r="2" spans="1:6">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="5"/>
+      <c r="F2" s="2"/>
     </row>
-    <row r="3">
-      <c r="A3" s="7" t="s">
+    <row r="3" spans="1:6">
+      <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="C3">
+        <v>1575</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="8">
-        <v>2022.0</v>
+      <c r="F3" s="10">
+        <v>44562</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="7" t="s">
+    <row r="4" spans="1:6">
+      <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="C4">
+        <v>1400</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="8">
-        <v>2022.0</v>
+      <c r="F4" s="10">
+        <v>44593</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="7" t="s">
+    <row r="5" spans="1:6" ht="30">
+      <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="C5">
+        <v>855</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="8">
-        <v>2022.0</v>
+      <c r="F5" s="10">
+        <v>44682</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="7" t="s">
+    <row r="6" spans="1:6" ht="30">
+      <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="C6">
+        <v>286</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="8">
-        <v>2022.0</v>
+      <c r="F6" s="10">
+        <v>44652</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="9" t="s">
+    <row r="7" spans="1:6" ht="30">
+      <c r="A7" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="C7">
+        <v>148</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="8">
-        <v>2022.0</v>
+      <c r="F7" s="10">
+        <v>44652</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="9" t="s">
+    <row r="8" spans="1:6" ht="30">
+      <c r="A8" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="C8">
+        <v>4562</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="8">
-        <v>2022.0</v>
+      <c r="F8" s="10">
+        <v>44197</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="9" t="s">
+    <row r="9" spans="1:6" ht="30">
+      <c r="A9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="C9">
+        <v>454</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="8">
-        <v>2022.0</v>
+      <c r="F9" s="10">
+        <v>44531</v>
       </c>
     </row>
-    <row r="12" ht="15.75" customHeight="1"/>
-    <row r="13" ht="15.75" customHeight="1"/>
-    <row r="14" ht="15.75" customHeight="1"/>
-    <row r="15" ht="15.75" customHeight="1"/>
-    <row r="16" ht="15.75" customHeight="1"/>
+    <row r="12" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="13" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="14" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="15" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="16" spans="1:6" ht="15.75" customHeight="1"/>
     <row r="17" ht="15.75" customHeight="1"/>
     <row r="18" ht="15.75" customHeight="1"/>
     <row r="19" ht="15.75" customHeight="1"/>
@@ -1546,9 +1599,7 @@
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:D1"/>
   </mergeCells>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
se corrigen mediciones 1 y 5
</commit_message>
<xml_diff>
--- a/mediciones4.xlsx
+++ b/mediciones4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Datos\UTN 2022\DDS 2022\DDS-2022-K3002-HuellaCarbonoG3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C31ADCB-BB5B-48BD-9597-E294B4E5AE0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8AF086D-A33C-46A8-877B-72D66E91DC5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -203,6 +203,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="17" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -211,7 +212,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="17" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -430,7 +430,7 @@
   <dimension ref="A1:F991"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -444,24 +444,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9"/>
+      <c r="D1" s="10"/>
       <c r="E1" s="1"/>
       <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
       <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
@@ -480,18 +480,13 @@
       <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C3">
-        <v>1575</v>
-      </c>
       <c r="D3" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="10">
-        <v>44562</v>
-      </c>
+      <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="3" t="s">
@@ -500,18 +495,13 @@
       <c r="B4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C4">
-        <v>1400</v>
-      </c>
       <c r="D4" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="10">
-        <v>44593</v>
-      </c>
+      <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:6" ht="30">
       <c r="A5" s="3" t="s">
@@ -520,18 +510,13 @@
       <c r="B5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C5">
-        <v>855</v>
-      </c>
       <c r="D5" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="10">
-        <v>44682</v>
-      </c>
+      <c r="F5" s="6"/>
     </row>
     <row r="6" spans="1:6" ht="30">
       <c r="A6" s="3" t="s">
@@ -540,18 +525,13 @@
       <c r="B6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C6">
-        <v>286</v>
-      </c>
       <c r="D6" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="10">
-        <v>44652</v>
-      </c>
+      <c r="F6" s="6"/>
     </row>
     <row r="7" spans="1:6" ht="30">
       <c r="A7" s="5" t="s">
@@ -560,18 +540,13 @@
       <c r="B7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C7">
-        <v>148</v>
-      </c>
       <c r="D7" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="10">
-        <v>44652</v>
-      </c>
+      <c r="F7" s="6"/>
     </row>
     <row r="8" spans="1:6" ht="30">
       <c r="A8" s="5" t="s">
@@ -580,18 +555,13 @@
       <c r="B8" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C8">
-        <v>4562</v>
-      </c>
       <c r="D8" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="10">
-        <v>44197</v>
-      </c>
+      <c r="F8" s="6"/>
     </row>
     <row r="9" spans="1:6" ht="30">
       <c r="A9" s="5" t="s">
@@ -600,18 +570,13 @@
       <c r="B9" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C9">
-        <v>454</v>
-      </c>
       <c r="D9" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="10">
-        <v>44531</v>
-      </c>
+      <c r="F9" s="6"/>
     </row>
     <row r="12" spans="1:6" ht="15.75" customHeight="1"/>
     <row r="13" spans="1:6" ht="15.75" customHeight="1"/>

</xml_diff>